<commit_message>
+ fixed labels, table, added contact
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,129 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valer\PycharmProjects\dashProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9220762C-E9C6-4352-A9A8-A23AD8F243DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B479754-F80F-4770-B19E-5E6FD12BA4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{61545F2E-B864-42A0-8651-7E577F359C43}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Зависимые выборки" sheetId="1" r:id="rId1"/>
     <sheet name="Независимые выборки" sheetId="2" r:id="rId2"/>
     <sheet name="Правила составления таблиц" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t xml:space="preserve">ОСНОВНЫЕ ПРАВИЛА СОСТАВЛЕНИЯ ТАБЛИЦ </t>
+    <t xml:space="preserve"> Группа 1</t>
   </si>
   <si>
-    <t>1. В первой строке должны находиться заголовки столбцов с разными контрольными группами для их выбора в системе расчета доверительного интервала разности медиан</t>
-  </si>
-  <si>
-    <t>2. Необходимо убедиться, что форматы ячеек с данными должны иметь числовой формат</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Для зависимых выборок</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: каждое значение первой контрольной группы должно иметь одно значений из второй контрольной группы, следовательно, объем данных должен совпадать в каждой группе (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>в нашем приложении есть возможность удалить записи с отсутствующими значениями в одной их групп</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>4. У вас есть возможность загрузить несколько столбцов данных и в дальнейшем выбрать их в приложении для исследования (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>главное, чтобы каждый столбец имел заголовок</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
+    <t>Группа 2</t>
   </si>
   <si>
     <t>ИМТ до</t>
@@ -132,34 +41,11 @@
     <t>ИМТ после</t>
   </si>
   <si>
-    <t>6. Убедитесь, что размер файла не превышает 2 МБ</t>
-  </si>
-  <si>
-    <t>5. Таблица должна находиться в первом листе файла</t>
+    <t xml:space="preserve"> ТРЕБОВАНИЯ К ТАБЛИЦЕ ЗАГРУЖАЕМЫХ ДАННЫХ</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Источник для составления примеров таблиц данных:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> статья </t>
+      <t xml:space="preserve">Пример данных взят из статьи </t>
     </r>
     <r>
       <rPr>
@@ -186,10 +72,106 @@
     </r>
   </si>
   <si>
-    <t>ИМТ</t>
+    <t>Размер файла не должен превышать 2 МБ</t>
   </si>
   <si>
-    <t>Группа</t>
+    <t>Ограничений для количества столбцов в загружаемом файле нет</t>
+  </si>
+  <si>
+    <t>Данные для загрузки из Таблицы Excel должны находиться на первом листе файла</t>
+  </si>
+  <si>
+    <t>Ячейки с данными должны иметь числовой формат</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Первая строка должна содержать заголовки столбцов/переменных </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Для 2-х зависимых выборок</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: количество непустых строк должно совпадать в обоих столбцах (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>в нашем приложении есть возможность удалить записи с отсутствующими значениями</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Для 2-х независимых выборок: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> количество строк для каждого столбца может </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>не совпадать.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -284,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +276,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,31 +313,33 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="2" xr:uid="{276FA841-A98B-405D-B8E8-3CC59855EEB5}"/>
-    <cellStyle name="Обычный 3" xfId="3" xr:uid="{A5AFFCC6-C086-4EAA-BDA4-3E68CD808D7B}"/>
-    <cellStyle name="Обычный_Лист1" xfId="1" xr:uid="{0BBF33D6-7EFF-40AB-8CE1-B314DD7FAC81}"/>
+    <cellStyle name="Обычный 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Обычный_Лист1" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -660,11 +650,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB44D742-7D90-49D3-A08E-3762530B50E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,10 +664,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1224,25 +1214,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6312018E-244F-4BC5-9BFF-3C5AFF8B8740}">
-  <dimension ref="A1:AB67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1254,12 +1244,12 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>34.15</v>
       </c>
-      <c r="B2" s="14">
-        <v>1</v>
+      <c r="B2" s="3">
+        <v>23.7</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1287,600 +1277,351 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AC2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>32.96</v>
       </c>
-      <c r="B3" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B3" s="3">
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>26.13</v>
       </c>
-      <c r="B4" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B4" s="3">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>30.17</v>
       </c>
-      <c r="B5" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>25.93</v>
       </c>
-      <c r="B6" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>24.06</v>
       </c>
-      <c r="B7" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>25.7</v>
       </c>
-      <c r="B8" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>28.73</v>
       </c>
-      <c r="B9" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>25.46</v>
       </c>
-      <c r="B10" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>29.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>25.06</v>
       </c>
-      <c r="B11" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>25.31</v>
       </c>
-      <c r="B12" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>27.32</v>
       </c>
-      <c r="B13" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>24.41</v>
       </c>
-      <c r="B14" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>26.62</v>
       </c>
-      <c r="B15" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>28.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>22.47</v>
       </c>
-      <c r="B16" s="15">
-        <v>1</v>
+      <c r="B16" s="3">
+        <v>27.3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>26.67</v>
       </c>
-      <c r="B17" s="15">
-        <v>0</v>
+      <c r="B17" s="3">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>23.47</v>
       </c>
-      <c r="B18" s="15">
-        <v>1</v>
+      <c r="B18" s="3">
+        <v>25.9</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>23.58</v>
       </c>
-      <c r="B19" s="15">
-        <v>1</v>
+      <c r="B19" s="3">
+        <v>28.3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>24.78</v>
       </c>
-      <c r="B20" s="15">
-        <v>0</v>
+      <c r="B20" s="3">
+        <v>28.4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>27.25</v>
       </c>
-      <c r="B21" s="15">
-        <v>0</v>
+      <c r="B21" s="3">
+        <v>28.5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>24.06</v>
       </c>
-      <c r="B22" s="15">
-        <v>0</v>
+      <c r="B22" s="3">
+        <v>27.8</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>25</v>
       </c>
-      <c r="B23" s="15">
-        <v>0</v>
+      <c r="B23" s="3">
+        <v>30.1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>25.25</v>
       </c>
-      <c r="B24" s="15">
-        <v>0</v>
+      <c r="B24" s="3">
+        <v>29.4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>21.22</v>
       </c>
-      <c r="B25" s="15">
-        <v>1</v>
+      <c r="B25" s="3">
+        <v>29.2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>26.09</v>
       </c>
-      <c r="B26" s="15">
-        <v>1</v>
+      <c r="B26" s="3">
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>24.86</v>
       </c>
-      <c r="B27" s="15">
-        <v>0</v>
+      <c r="B27" s="3">
+        <v>26.6</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>25.32</v>
       </c>
-      <c r="B28" s="15">
-        <v>0</v>
+      <c r="B28" s="3">
+        <v>28.2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>25.1</v>
       </c>
-      <c r="B29" s="15">
-        <v>0</v>
+      <c r="B29" s="3">
+        <v>25.8</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>24.24</v>
       </c>
-      <c r="B30" s="15">
-        <v>0</v>
-      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>22.02</v>
       </c>
-      <c r="B31" s="15">
-        <v>0</v>
-      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>25.18</v>
       </c>
-      <c r="B32" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>21.29</v>
       </c>
-      <c r="B33" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>23.98</v>
       </c>
-      <c r="B34" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>21.64</v>
       </c>
-      <c r="B35" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>23.7</v>
       </c>
-      <c r="B36" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>21.66</v>
       </c>
-      <c r="B37" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>19.989999999999998</v>
       </c>
-      <c r="B38" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>20.89</v>
       </c>
-      <c r="B39" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="3">
-        <v>23.7</v>
-      </c>
-      <c r="B40" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="3">
-        <v>30.3</v>
-      </c>
-      <c r="B41" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="3">
-        <v>31.4</v>
-      </c>
-      <c r="B42" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="3">
-        <v>28</v>
-      </c>
-      <c r="B43" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="B44" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="3">
-        <v>28.7</v>
-      </c>
-      <c r="B45" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="3">
-        <v>27.8</v>
-      </c>
-      <c r="B46" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="3">
-        <v>26.5</v>
-      </c>
-      <c r="B47" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="3">
-        <v>29.4</v>
-      </c>
-      <c r="B48" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="3">
-        <v>28</v>
-      </c>
-      <c r="B49" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="3">
-        <v>36.5</v>
-      </c>
-      <c r="B50" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="3">
-        <v>25.7</v>
-      </c>
-      <c r="B51" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="3">
-        <v>26.6</v>
-      </c>
-      <c r="B52" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="3">
-        <v>28.4</v>
-      </c>
-      <c r="B53" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="3">
-        <v>27.3</v>
-      </c>
-      <c r="B54" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="3">
-        <v>28</v>
-      </c>
-      <c r="B55" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="3">
-        <v>25.9</v>
-      </c>
-      <c r="B56" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="3">
-        <v>28.3</v>
-      </c>
-      <c r="B57" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="3">
-        <v>28.4</v>
-      </c>
-      <c r="B58" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="3">
-        <v>28.5</v>
-      </c>
-      <c r="B59" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="3">
-        <v>27.8</v>
-      </c>
-      <c r="B60" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="3">
-        <v>30.1</v>
-      </c>
-      <c r="B61" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="3">
-        <v>29.4</v>
-      </c>
-      <c r="B62" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="3">
-        <v>29.2</v>
-      </c>
-      <c r="B63" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="3">
-        <v>31</v>
-      </c>
-      <c r="B64" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="3">
-        <v>26.6</v>
-      </c>
-      <c r="B65" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="3">
-        <v>28.2</v>
-      </c>
-      <c r="B66" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="3">
-        <v>25.8</v>
-      </c>
-      <c r="B67" s="15">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050A557C-4CC5-4D44-90D2-7DCFCB710049}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
+      <c r="A3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="A4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -1892,8 +1633,10 @@
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -1905,168 +1648,168 @@
       <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="A13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A13:J18"/>
-    <mergeCell ref="A5:J8"/>
-    <mergeCell ref="A9:J10"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A6:J6"/>
     <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A8:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>